<commit_message>
New test case that shows that words which style is changed at midword are returned cut in two parts.
</commit_message>
<xml_diff>
--- a/tests/in/spreadsheet1.xlsx
+++ b/tests/in/spreadsheet1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="420" windowWidth="21600" windowHeight="12980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="14580"/>
   </bookViews>
   <sheets>
     <sheet name="First sheet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>this</t>
   </si>
@@ -32,22 +32,47 @@
     <t>a</t>
   </si>
   <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>another</t>
+  </si>
+  <si>
     <t>spreadsheet</t>
   </si>
   <si>
-    <t>this</t>
-  </si>
-  <si>
-    <t>is</t>
-  </si>
-  <si>
-    <t>another</t>
-  </si>
-  <si>
-    <t>spreadsheet</t>
-  </si>
-  <si>
     <t>A sum</t>
+  </si>
+  <si>
+    <r>
+      <t>spread</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>sheet</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>mid</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>word</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -55,9 +80,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-40C];[Red]\-#,##0.00\ [$€-40C]"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C];[Red]\-#,##0.00\ [$€-40C]"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -83,6 +108,11 @@
       <sz val="8"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,7 +135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -450,18 +480,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="13" customHeight="1"/>
   <cols>
     <col min="1" max="5" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75">
+    <row r="1" spans="1:5" ht="12.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +500,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -506,19 +537,20 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.75">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
@@ -561,10 +593,11 @@
         <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>

</xml_diff>